<commit_message>
fix(firmware): add sig mesh & zigbee dual mode document.
</commit_message>
<xml_diff>
--- a/doc/SigmeshZigbeeFlashmapNormal.xlsx
+++ b/doc/SigmeshZigbeeFlashmapNormal.xlsx
@@ -1,29 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\BLE\客户\amazon\文档\flash_map\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\git_lab\release_sdk\telink_sig_mesh_sdk\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACC39206-2F3E-46FC-9B11-9350BBF5AE64}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9750"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DualMode_1M_0402" sheetId="11" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -255,9 +250,6 @@
     <t xml:space="preserve">NV_MODULE_APP </t>
   </si>
   <si>
-    <t>NV_MODULE_KEYPAIR</t>
-  </si>
-  <si>
     <t>…</t>
   </si>
   <si>
@@ -335,13 +327,17 @@
   </si>
   <si>
     <t>Telink Mac</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>NV_MODULE_KEYPAIR</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -751,6 +747,159 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -760,64 +909,262 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -826,96 +1173,30 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -940,322 +1221,37 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="25" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="25" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="25" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="25" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="26" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="26" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="26" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="26" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="常规 2" xfId="1"/>
+    <cellStyle name="常规 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1566,11 +1562,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X57"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" zoomScale="74" zoomScaleNormal="74" workbookViewId="0">
-      <selection activeCell="Q23" sqref="Q23:Q25"/>
+      <selection activeCell="V34" sqref="V34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1603,10 +1599,10 @@
       <c r="A1" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="177" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="37"/>
+      <c r="C1" s="177"/>
       <c r="D1" s="12" t="s">
         <v>10</v>
       </c>
@@ -1616,20 +1612,20 @@
       <c r="H1" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="37" t="s">
+      <c r="I1" s="177" t="s">
         <v>14</v>
       </c>
-      <c r="J1" s="37"/>
+      <c r="J1" s="177"/>
       <c r="K1" s="12" t="s">
         <v>10</v>
       </c>
       <c r="M1" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="N1" s="37" t="s">
+      <c r="N1" s="177" t="s">
         <v>14</v>
       </c>
-      <c r="O1" s="37"/>
+      <c r="O1" s="177"/>
       <c r="P1" s="12" t="s">
         <v>10</v>
       </c>
@@ -1639,10 +1635,10 @@
       <c r="U1" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="V1" s="37" t="s">
+      <c r="V1" s="177" t="s">
         <v>14</v>
       </c>
-      <c r="W1" s="37"/>
+      <c r="W1" s="177"/>
       <c r="X1" s="12" t="s">
         <v>10</v>
       </c>
@@ -1651,47 +1647,47 @@
       <c r="A2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="75" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="22">
+      <c r="C2" s="75"/>
+      <c r="D2" s="29">
         <v>192</v>
       </c>
-      <c r="E2" s="18"/>
+      <c r="E2" s="55"/>
       <c r="H2" s="5" t="str">
         <f>M23</f>
         <v>26000</v>
       </c>
-      <c r="I2" s="70" t="s">
+      <c r="I2" s="165" t="s">
         <v>33</v>
       </c>
-      <c r="J2" s="71"/>
-      <c r="K2" s="63">
+      <c r="J2" s="166"/>
+      <c r="K2" s="37">
         <v>4</v>
       </c>
       <c r="M2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="N2" s="39" t="s">
-        <v>67</v>
-      </c>
-      <c r="O2" s="39"/>
-      <c r="P2" s="22">
+      <c r="N2" s="156" t="s">
+        <v>66</v>
+      </c>
+      <c r="O2" s="156"/>
+      <c r="P2" s="29">
         <v>24</v>
       </c>
-      <c r="Q2" s="167" t="s">
+      <c r="Q2" s="163" t="s">
         <v>27</v>
       </c>
       <c r="U2" s="5" t="str">
         <f>M23</f>
         <v>26000</v>
       </c>
-      <c r="V2" s="70" t="s">
+      <c r="V2" s="165" t="s">
         <v>54</v>
       </c>
-      <c r="W2" s="71"/>
-      <c r="X2" s="63">
+      <c r="W2" s="166"/>
+      <c r="X2" s="37">
         <v>8</v>
       </c>
     </row>
@@ -1699,110 +1695,110 @@
       <c r="A3" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="18"/>
+      <c r="B3" s="75"/>
+      <c r="C3" s="75"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="55"/>
       <c r="H3" s="7" t="str">
         <f>DEC2HEX(HEX2DEC(H2)+K2*1024 - 1)</f>
         <v>26FFF</v>
       </c>
-      <c r="I3" s="74"/>
-      <c r="J3" s="75"/>
-      <c r="K3" s="64"/>
+      <c r="I3" s="169"/>
+      <c r="J3" s="170"/>
+      <c r="K3" s="38"/>
       <c r="M3" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="N3" s="39"/>
-      <c r="O3" s="39"/>
-      <c r="P3" s="22"/>
-      <c r="Q3" s="45"/>
+      <c r="N3" s="156"/>
+      <c r="O3" s="156"/>
+      <c r="P3" s="29"/>
+      <c r="Q3" s="164"/>
       <c r="U3" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="V3" s="72"/>
-      <c r="W3" s="73"/>
-      <c r="X3" s="69"/>
+        <v>61</v>
+      </c>
+      <c r="V3" s="167"/>
+      <c r="W3" s="168"/>
+      <c r="X3" s="118"/>
     </row>
     <row r="4" spans="1:24" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="str">
         <f>DEC2HEX(HEX2DEC(A2)+D2*1024 - 1)</f>
         <v>2FFFF</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="18"/>
+      <c r="B4" s="75"/>
+      <c r="C4" s="75"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="55"/>
       <c r="H4" s="8" t="str">
         <f>DEC2HEX(HEX2DEC(H3)+1)</f>
         <v>27000</v>
       </c>
-      <c r="I4" s="76" t="s">
+      <c r="I4" s="171" t="s">
         <v>34</v>
       </c>
-      <c r="J4" s="77"/>
-      <c r="K4" s="63">
+      <c r="J4" s="172"/>
+      <c r="K4" s="37">
         <v>4</v>
       </c>
       <c r="M4" s="7" t="str">
         <f>DEC2HEX(HEX2DEC(M2)+P2*1024 - 1)</f>
         <v>5FFF</v>
       </c>
-      <c r="N4" s="39"/>
-      <c r="O4" s="39"/>
-      <c r="P4" s="22"/>
-      <c r="Q4" s="45"/>
+      <c r="N4" s="156"/>
+      <c r="O4" s="156"/>
+      <c r="P4" s="29"/>
+      <c r="Q4" s="164"/>
       <c r="U4" s="7" t="str">
         <f>DEC2HEX(HEX2DEC(U2)+X2*1024 - 1)</f>
         <v>27FFF</v>
       </c>
-      <c r="V4" s="74"/>
-      <c r="W4" s="75"/>
-      <c r="X4" s="64"/>
+      <c r="V4" s="169"/>
+      <c r="W4" s="170"/>
+      <c r="X4" s="38"/>
     </row>
     <row r="5" spans="1:24" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="str">
         <f>DEC2HEX(HEX2DEC(A4)+1)</f>
         <v>30000</v>
       </c>
-      <c r="B5" s="40" t="s">
+      <c r="B5" s="178" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="41"/>
-      <c r="D5" s="22">
+      <c r="C5" s="179"/>
+      <c r="D5" s="29">
         <v>64</v>
       </c>
-      <c r="E5" s="18"/>
+      <c r="E5" s="55"/>
       <c r="H5" s="9" t="str">
         <f>DEC2HEX(HEX2DEC(H4)+K4*1024 - 1)</f>
         <v>27FFF</v>
       </c>
-      <c r="I5" s="80"/>
-      <c r="J5" s="81"/>
-      <c r="K5" s="64"/>
+      <c r="I5" s="173"/>
+      <c r="J5" s="174"/>
+      <c r="K5" s="38"/>
       <c r="M5" s="8" t="str">
         <f>DEC2HEX(HEX2DEC(M4)+1)</f>
         <v>6000</v>
       </c>
-      <c r="N5" s="168" t="s">
-        <v>81</v>
-      </c>
-      <c r="O5" s="101"/>
-      <c r="P5" s="31">
-        <v>4</v>
-      </c>
-      <c r="Q5" s="169" t="s">
-        <v>77</v>
+      <c r="N5" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="O5" s="16"/>
+      <c r="P5" s="21">
+        <v>4</v>
+      </c>
+      <c r="Q5" s="24" t="s">
+        <v>76</v>
       </c>
       <c r="U5" s="8" t="str">
         <f>DEC2HEX(HEX2DEC(U4)+1)</f>
         <v>28000</v>
       </c>
-      <c r="V5" s="76" t="s">
+      <c r="V5" s="171" t="s">
         <v>55</v>
       </c>
-      <c r="W5" s="77"/>
-      <c r="X5" s="63">
+      <c r="W5" s="172"/>
+      <c r="X5" s="37">
         <v>8</v>
       </c>
     </row>
@@ -1810,114 +1806,114 @@
       <c r="A6" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="42"/>
-      <c r="C6" s="43"/>
-      <c r="D6" s="22"/>
-      <c r="E6" s="18"/>
+      <c r="B6" s="180"/>
+      <c r="C6" s="181"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="55"/>
       <c r="H6" s="8" t="str">
         <f t="shared" ref="H6" si="0">DEC2HEX(HEX2DEC(H5)+1)</f>
         <v>28000</v>
       </c>
-      <c r="I6" s="82" t="s">
+      <c r="I6" s="143" t="s">
         <v>35</v>
       </c>
-      <c r="J6" s="83"/>
-      <c r="K6" s="63">
+      <c r="J6" s="144"/>
+      <c r="K6" s="37">
         <v>4</v>
       </c>
       <c r="M6" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="N6" s="102"/>
-      <c r="O6" s="103"/>
-      <c r="P6" s="32"/>
-      <c r="Q6" s="47"/>
+      <c r="N6" s="17"/>
+      <c r="O6" s="18"/>
+      <c r="P6" s="22"/>
+      <c r="Q6" s="25"/>
       <c r="U6" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="V6" s="78"/>
-      <c r="W6" s="79"/>
-      <c r="X6" s="69"/>
+        <v>61</v>
+      </c>
+      <c r="V6" s="175"/>
+      <c r="W6" s="176"/>
+      <c r="X6" s="118"/>
     </row>
     <row r="7" spans="1:24" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="e">
         <f>DEC2HEX(HEX2DEC(#REF!)+#REF!*1024 - 1)</f>
         <v>#REF!</v>
       </c>
-      <c r="B7" s="21"/>
-      <c r="C7" s="21"/>
+      <c r="B7" s="30"/>
+      <c r="C7" s="30"/>
       <c r="D7" s="13"/>
       <c r="E7" s="14"/>
       <c r="H7" s="9" t="str">
         <f>DEC2HEX(HEX2DEC(H6)+K6*1024 - 1)</f>
         <v>28FFF</v>
       </c>
-      <c r="I7" s="86"/>
-      <c r="J7" s="87"/>
-      <c r="K7" s="64"/>
+      <c r="I7" s="145"/>
+      <c r="J7" s="146"/>
+      <c r="K7" s="38"/>
       <c r="M7" s="9" t="str">
         <f>DEC2HEX(HEX2DEC(M5)+P5*1024 - 1)</f>
         <v>6FFF</v>
       </c>
-      <c r="N7" s="104"/>
-      <c r="O7" s="105"/>
-      <c r="P7" s="33"/>
-      <c r="Q7" s="48"/>
+      <c r="N7" s="19"/>
+      <c r="O7" s="20"/>
+      <c r="P7" s="23"/>
+      <c r="Q7" s="26"/>
       <c r="U7" s="9" t="str">
         <f>DEC2HEX(HEX2DEC(U5)+X5*1024 - 1)</f>
         <v>29FFF</v>
       </c>
-      <c r="V7" s="80"/>
-      <c r="W7" s="81"/>
-      <c r="X7" s="64"/>
+      <c r="V7" s="173"/>
+      <c r="W7" s="174"/>
+      <c r="X7" s="38"/>
     </row>
     <row r="8" spans="1:24" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="e">
         <f t="shared" ref="A8" si="1">DEC2HEX(HEX2DEC(A7)+1)</f>
         <v>#REF!</v>
       </c>
-      <c r="B8" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="38"/>
-      <c r="D8" s="22">
+      <c r="B8" s="155" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="155"/>
+      <c r="D8" s="29">
         <v>256</v>
       </c>
-      <c r="E8" s="18"/>
+      <c r="E8" s="55"/>
       <c r="H8" s="8" t="str">
         <f t="shared" ref="H8" si="2">DEC2HEX(HEX2DEC(H7)+1)</f>
         <v>29000</v>
       </c>
-      <c r="I8" s="88" t="s">
+      <c r="I8" s="149" t="s">
         <v>36</v>
       </c>
-      <c r="J8" s="89"/>
-      <c r="K8" s="63">
+      <c r="J8" s="150"/>
+      <c r="K8" s="37">
         <v>4</v>
       </c>
       <c r="M8" s="8" t="str">
         <f t="shared" ref="M8" si="3">DEC2HEX(HEX2DEC(M7)+1)</f>
         <v>7000</v>
       </c>
-      <c r="N8" s="165" t="s">
-        <v>79</v>
-      </c>
-      <c r="O8" s="166"/>
-      <c r="P8" s="22">
-        <v>4</v>
-      </c>
-      <c r="Q8" s="46" t="s">
+      <c r="N8" s="27" t="s">
         <v>78</v>
+      </c>
+      <c r="O8" s="28"/>
+      <c r="P8" s="29">
+        <v>4</v>
+      </c>
+      <c r="Q8" s="32" t="s">
+        <v>77</v>
       </c>
       <c r="U8" s="8" t="str">
         <f t="shared" ref="U8" si="4">DEC2HEX(HEX2DEC(U7)+1)</f>
         <v>2A000</v>
       </c>
-      <c r="V8" s="82" t="s">
+      <c r="V8" s="143" t="s">
         <v>56</v>
       </c>
-      <c r="W8" s="83"/>
-      <c r="X8" s="63">
+      <c r="W8" s="144"/>
+      <c r="X8" s="37">
         <v>8</v>
       </c>
     </row>
@@ -1925,112 +1921,112 @@
       <c r="A9" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="38"/>
-      <c r="C9" s="38"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="18"/>
+      <c r="B9" s="155"/>
+      <c r="C9" s="155"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="55"/>
       <c r="H9" s="9" t="str">
         <f>DEC2HEX(HEX2DEC(H8)+K8*1024 - 1)</f>
         <v>29FFF</v>
       </c>
-      <c r="I9" s="92"/>
-      <c r="J9" s="93"/>
-      <c r="K9" s="64"/>
+      <c r="I9" s="153"/>
+      <c r="J9" s="154"/>
+      <c r="K9" s="38"/>
       <c r="M9" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="N9" s="166"/>
-      <c r="O9" s="166"/>
-      <c r="P9" s="22"/>
-      <c r="Q9" s="47"/>
+      <c r="N9" s="28"/>
+      <c r="O9" s="28"/>
+      <c r="P9" s="29"/>
+      <c r="Q9" s="25"/>
       <c r="U9" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="V9" s="84"/>
-      <c r="W9" s="85"/>
-      <c r="X9" s="69"/>
+        <v>61</v>
+      </c>
+      <c r="V9" s="147"/>
+      <c r="W9" s="148"/>
+      <c r="X9" s="118"/>
     </row>
     <row r="10" spans="1:24" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="e">
         <f t="shared" ref="A10" si="5">DEC2HEX(HEX2DEC(A8)+D8*1024 - 1)</f>
         <v>#REF!</v>
       </c>
-      <c r="B10" s="38"/>
-      <c r="C10" s="38"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="18"/>
+      <c r="B10" s="155"/>
+      <c r="C10" s="155"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="55"/>
       <c r="H10" s="8" t="str">
         <f t="shared" ref="H10" si="6">DEC2HEX(HEX2DEC(H9)+1)</f>
         <v>2A000</v>
       </c>
-      <c r="I10" s="94" t="s">
+      <c r="I10" s="136" t="s">
         <v>37</v>
       </c>
-      <c r="J10" s="95"/>
-      <c r="K10" s="63">
+      <c r="J10" s="137"/>
+      <c r="K10" s="37">
         <v>4</v>
       </c>
       <c r="M10" s="9" t="str">
         <f t="shared" ref="M10" si="7">DEC2HEX(HEX2DEC(M8)+P8*1024 - 1)</f>
         <v>7FFF</v>
       </c>
-      <c r="N10" s="166"/>
-      <c r="O10" s="166"/>
-      <c r="P10" s="22"/>
-      <c r="Q10" s="48"/>
+      <c r="N10" s="28"/>
+      <c r="O10" s="28"/>
+      <c r="P10" s="29"/>
+      <c r="Q10" s="26"/>
       <c r="U10" s="9" t="str">
         <f>DEC2HEX(HEX2DEC(U8)+X8*1024 - 1)</f>
         <v>2BFFF</v>
       </c>
-      <c r="V10" s="86"/>
-      <c r="W10" s="87"/>
-      <c r="X10" s="64"/>
+      <c r="V10" s="145"/>
+      <c r="W10" s="146"/>
+      <c r="X10" s="38"/>
     </row>
     <row r="11" spans="1:24" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="e">
         <f t="shared" ref="A11" si="8">DEC2HEX(HEX2DEC(A10)+1)</f>
         <v>#REF!</v>
       </c>
-      <c r="B11" s="39" t="s">
+      <c r="B11" s="156" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="39"/>
-      <c r="D11" s="22">
+      <c r="C11" s="156"/>
+      <c r="D11" s="29">
         <v>128</v>
       </c>
-      <c r="E11" s="18" t="s">
+      <c r="E11" s="55" t="s">
         <v>23</v>
       </c>
       <c r="H11" s="9" t="str">
         <f>DEC2HEX(HEX2DEC(H10)+K10*1024 - 1)</f>
         <v>2AFFF</v>
       </c>
-      <c r="I11" s="98"/>
-      <c r="J11" s="99"/>
-      <c r="K11" s="64"/>
+      <c r="I11" s="140"/>
+      <c r="J11" s="141"/>
+      <c r="K11" s="38"/>
       <c r="M11" s="8" t="str">
         <f t="shared" ref="M11" si="9">DEC2HEX(HEX2DEC(M10)+1)</f>
         <v>8000</v>
       </c>
-      <c r="N11" s="176" t="s">
-        <v>80</v>
-      </c>
-      <c r="O11" s="177"/>
-      <c r="P11" s="31">
+      <c r="N11" s="157" t="s">
+        <v>79</v>
+      </c>
+      <c r="O11" s="158"/>
+      <c r="P11" s="21">
         <v>108</v>
       </c>
-      <c r="Q11" s="46" t="s">
-        <v>78</v>
+      <c r="Q11" s="32" t="s">
+        <v>77</v>
       </c>
       <c r="U11" s="8" t="str">
         <f t="shared" ref="U11" si="10">DEC2HEX(HEX2DEC(U10)+1)</f>
         <v>2C000</v>
       </c>
-      <c r="V11" s="88" t="s">
+      <c r="V11" s="149" t="s">
         <v>57</v>
       </c>
-      <c r="W11" s="89"/>
-      <c r="X11" s="63">
+      <c r="W11" s="150"/>
+      <c r="X11" s="37">
         <v>8</v>
       </c>
     </row>
@@ -2038,118 +2034,118 @@
       <c r="A12" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="39"/>
-      <c r="C12" s="39"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="18"/>
+      <c r="B12" s="156"/>
+      <c r="C12" s="156"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="55"/>
       <c r="H12" s="8" t="str">
         <f t="shared" ref="H12" si="11">DEC2HEX(HEX2DEC(H11)+1)</f>
         <v>2B000</v>
       </c>
-      <c r="I12" s="100" t="s">
+      <c r="I12" s="142" t="s">
         <v>38</v>
       </c>
-      <c r="J12" s="101"/>
-      <c r="K12" s="63">
+      <c r="J12" s="16"/>
+      <c r="K12" s="37">
         <v>4</v>
       </c>
       <c r="M12" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="N12" s="178"/>
-      <c r="O12" s="179"/>
-      <c r="P12" s="32"/>
-      <c r="Q12" s="47"/>
+      <c r="N12" s="159"/>
+      <c r="O12" s="160"/>
+      <c r="P12" s="22"/>
+      <c r="Q12" s="25"/>
       <c r="U12" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="V12" s="90"/>
-      <c r="W12" s="91"/>
-      <c r="X12" s="69"/>
+        <v>61</v>
+      </c>
+      <c r="V12" s="151"/>
+      <c r="W12" s="152"/>
+      <c r="X12" s="118"/>
     </row>
     <row r="13" spans="1:24" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="e">
         <f t="shared" ref="A13" si="12">DEC2HEX(HEX2DEC(A11)+D11*1024 - 1)</f>
         <v>#REF!</v>
       </c>
-      <c r="B13" s="39"/>
-      <c r="C13" s="39"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="18"/>
+      <c r="B13" s="156"/>
+      <c r="C13" s="156"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="55"/>
       <c r="H13" s="9" t="str">
         <f>DEC2HEX(HEX2DEC(H12)+K12*1024 - 1)</f>
         <v>2BFFF</v>
       </c>
-      <c r="I13" s="104"/>
-      <c r="J13" s="105"/>
-      <c r="K13" s="64"/>
+      <c r="I13" s="19"/>
+      <c r="J13" s="20"/>
+      <c r="K13" s="38"/>
       <c r="M13" s="9" t="str">
         <f t="shared" ref="M13" si="13">DEC2HEX(HEX2DEC(M11)+P11*1024 - 1)</f>
         <v>22FFF</v>
       </c>
-      <c r="N13" s="180"/>
-      <c r="O13" s="181"/>
-      <c r="P13" s="33"/>
-      <c r="Q13" s="48"/>
+      <c r="N13" s="161"/>
+      <c r="O13" s="162"/>
+      <c r="P13" s="23"/>
+      <c r="Q13" s="26"/>
       <c r="U13" s="9" t="str">
         <f>DEC2HEX(HEX2DEC(U11)+X11*1024 - 1)</f>
         <v>2DFFF</v>
       </c>
-      <c r="V13" s="92"/>
-      <c r="W13" s="93"/>
-      <c r="X13" s="64"/>
+      <c r="V13" s="153"/>
+      <c r="W13" s="154"/>
+      <c r="X13" s="38"/>
     </row>
     <row r="14" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="e">
         <f t="shared" ref="A14" si="14">DEC2HEX(HEX2DEC(A13)+1)</f>
         <v>#REF!</v>
       </c>
-      <c r="B14" s="20" t="s">
+      <c r="B14" s="75" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="21" t="s">
+      <c r="C14" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="22">
+      <c r="D14" s="29">
         <v>88</v>
       </c>
-      <c r="E14" s="18"/>
+      <c r="E14" s="55"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="8" t="str">
         <f t="shared" ref="H14" si="15">DEC2HEX(HEX2DEC(H13)+1)</f>
         <v>2C000</v>
       </c>
-      <c r="I14" s="114" t="s">
+      <c r="I14" s="112" t="s">
         <v>39</v>
       </c>
-      <c r="J14" s="115"/>
-      <c r="K14" s="63">
+      <c r="J14" s="113"/>
+      <c r="K14" s="37">
         <v>4</v>
       </c>
       <c r="M14" s="8" t="str">
         <f t="shared" ref="M14:M44" si="16">DEC2HEX(HEX2DEC(M13)+1)</f>
         <v>23000</v>
       </c>
-      <c r="N14" s="110" t="s">
-        <v>68</v>
-      </c>
-      <c r="O14" s="111"/>
-      <c r="P14" s="31">
-        <v>4</v>
-      </c>
-      <c r="Q14" s="46" t="s">
-        <v>70</v>
+      <c r="N14" s="90" t="s">
+        <v>67</v>
+      </c>
+      <c r="O14" s="91"/>
+      <c r="P14" s="21">
+        <v>4</v>
+      </c>
+      <c r="Q14" s="32" t="s">
+        <v>69</v>
       </c>
       <c r="U14" s="8" t="str">
         <f t="shared" ref="U14" si="17">DEC2HEX(HEX2DEC(U13)+1)</f>
         <v>2E000</v>
       </c>
-      <c r="V14" s="94" t="s">
+      <c r="V14" s="136" t="s">
         <v>58</v>
       </c>
-      <c r="W14" s="95"/>
-      <c r="X14" s="63">
+      <c r="W14" s="137"/>
+      <c r="X14" s="37">
         <v>8</v>
       </c>
     </row>
@@ -2157,10 +2153,10 @@
       <c r="A15" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="20"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="22"/>
-      <c r="E15" s="18"/>
+      <c r="B15" s="75"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="29"/>
+      <c r="E15" s="55"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="9" t="str">
@@ -2169,106 +2165,106 @@
       </c>
       <c r="I15" s="116"/>
       <c r="J15" s="117"/>
-      <c r="K15" s="64"/>
+      <c r="K15" s="38"/>
       <c r="M15" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="N15" s="120"/>
-      <c r="O15" s="121"/>
-      <c r="P15" s="32"/>
-      <c r="Q15" s="47"/>
+      <c r="N15" s="92"/>
+      <c r="O15" s="93"/>
+      <c r="P15" s="22"/>
+      <c r="Q15" s="25"/>
       <c r="U15" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="V15" s="96"/>
-      <c r="W15" s="97"/>
-      <c r="X15" s="69"/>
+        <v>61</v>
+      </c>
+      <c r="V15" s="138"/>
+      <c r="W15" s="139"/>
+      <c r="X15" s="118"/>
     </row>
     <row r="16" spans="1:24" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A16" s="9" t="e">
         <f t="shared" ref="A16" si="18">DEC2HEX(HEX2DEC(A14)+D14*1024 - 1)</f>
         <v>#REF!</v>
       </c>
-      <c r="B16" s="20"/>
-      <c r="C16" s="21"/>
-      <c r="D16" s="22"/>
-      <c r="E16" s="18"/>
+      <c r="B16" s="75"/>
+      <c r="C16" s="30"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="55"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="8" t="str">
         <f>DEC2HEX(HEX2DEC(H15)+1)</f>
         <v>2D000</v>
       </c>
-      <c r="I16" s="110" t="s">
+      <c r="I16" s="90" t="s">
         <v>40</v>
       </c>
-      <c r="J16" s="111"/>
-      <c r="K16" s="63">
+      <c r="J16" s="91"/>
+      <c r="K16" s="37">
         <v>4</v>
       </c>
       <c r="M16" s="9" t="str">
         <f t="shared" ref="M16:M46" si="19">DEC2HEX(HEX2DEC(M14)+P14*1024 - 1)</f>
         <v>23FFF</v>
       </c>
-      <c r="N16" s="112"/>
-      <c r="O16" s="113"/>
-      <c r="P16" s="33"/>
-      <c r="Q16" s="48"/>
+      <c r="N16" s="94"/>
+      <c r="O16" s="95"/>
+      <c r="P16" s="23"/>
+      <c r="Q16" s="26"/>
       <c r="U16" s="9" t="str">
         <f>DEC2HEX(HEX2DEC(U14)+X14*1024 - 1)</f>
         <v>2FFFF</v>
       </c>
-      <c r="V16" s="98"/>
-      <c r="W16" s="99"/>
-      <c r="X16" s="64"/>
+      <c r="V16" s="140"/>
+      <c r="W16" s="141"/>
+      <c r="X16" s="38"/>
     </row>
     <row r="17" spans="1:24" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="e">
         <f t="shared" ref="A17" si="20">DEC2HEX(HEX2DEC(A16)+1)</f>
         <v>#REF!</v>
       </c>
-      <c r="B17" s="20" t="s">
+      <c r="B17" s="75" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="21" t="s">
+      <c r="C17" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="22">
-        <v>4</v>
-      </c>
-      <c r="E17" s="18"/>
+      <c r="D17" s="29">
+        <v>4</v>
+      </c>
+      <c r="E17" s="55"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="9" t="str">
         <f>DEC2HEX(HEX2DEC(H16)+K16*1024 - 1)</f>
         <v>2DFFF</v>
       </c>
-      <c r="I17" s="112"/>
-      <c r="J17" s="113"/>
-      <c r="K17" s="64"/>
+      <c r="I17" s="94"/>
+      <c r="J17" s="95"/>
+      <c r="K17" s="38"/>
       <c r="M17" s="8" t="str">
         <f t="shared" si="16"/>
         <v>24000</v>
       </c>
-      <c r="N17" s="110" t="s">
+      <c r="N17" s="90" t="s">
         <v>26</v>
       </c>
-      <c r="O17" s="111"/>
-      <c r="P17" s="31">
-        <v>4</v>
-      </c>
-      <c r="Q17" s="46" t="s">
-        <v>63</v>
+      <c r="O17" s="91"/>
+      <c r="P17" s="21">
+        <v>4</v>
+      </c>
+      <c r="Q17" s="32" t="s">
+        <v>62</v>
       </c>
       <c r="U17" s="8" t="str">
         <f t="shared" ref="U17" si="21">DEC2HEX(HEX2DEC(U16)+1)</f>
         <v>30000</v>
       </c>
-      <c r="V17" s="100" t="s">
+      <c r="V17" s="142" t="s">
         <v>59</v>
       </c>
-      <c r="W17" s="101"/>
-      <c r="X17" s="63">
+      <c r="W17" s="16"/>
+      <c r="X17" s="37">
         <v>8</v>
       </c>
     </row>
@@ -2276,122 +2272,122 @@
       <c r="A18" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B18" s="20"/>
-      <c r="C18" s="21"/>
-      <c r="D18" s="22"/>
-      <c r="E18" s="18"/>
+      <c r="B18" s="75"/>
+      <c r="C18" s="30"/>
+      <c r="D18" s="29"/>
+      <c r="E18" s="55"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="8" t="str">
         <f t="shared" ref="H18" si="22">DEC2HEX(HEX2DEC(H17)+1)</f>
         <v>2E000</v>
       </c>
-      <c r="I18" s="106" t="s">
+      <c r="I18" s="132" t="s">
         <v>41</v>
       </c>
-      <c r="J18" s="107"/>
-      <c r="K18" s="63">
+      <c r="J18" s="133"/>
+      <c r="K18" s="37">
         <v>4</v>
       </c>
       <c r="M18" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="N18" s="120"/>
-      <c r="O18" s="121"/>
-      <c r="P18" s="32"/>
-      <c r="Q18" s="47"/>
+      <c r="N18" s="92"/>
+      <c r="O18" s="93"/>
+      <c r="P18" s="22"/>
+      <c r="Q18" s="25"/>
       <c r="U18" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="V18" s="102"/>
-      <c r="W18" s="103"/>
-      <c r="X18" s="69"/>
+        <v>61</v>
+      </c>
+      <c r="V18" s="17"/>
+      <c r="W18" s="18"/>
+      <c r="X18" s="118"/>
     </row>
     <row r="19" spans="1:24" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A19" s="9" t="e">
         <f t="shared" ref="A19" si="23">DEC2HEX(HEX2DEC(A17)+D17*1024 - 1)</f>
         <v>#REF!</v>
       </c>
-      <c r="B19" s="20"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="22"/>
-      <c r="E19" s="18"/>
+      <c r="B19" s="75"/>
+      <c r="C19" s="30"/>
+      <c r="D19" s="29"/>
+      <c r="E19" s="55"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="9" t="str">
         <f>DEC2HEX(HEX2DEC(H18)+K18*1024 - 1)</f>
         <v>2EFFF</v>
       </c>
-      <c r="I19" s="108"/>
-      <c r="J19" s="109"/>
-      <c r="K19" s="64"/>
+      <c r="I19" s="134"/>
+      <c r="J19" s="135"/>
+      <c r="K19" s="38"/>
       <c r="M19" s="9" t="str">
         <f t="shared" si="19"/>
         <v>24FFF</v>
       </c>
-      <c r="N19" s="112"/>
-      <c r="O19" s="113"/>
-      <c r="P19" s="33"/>
-      <c r="Q19" s="48"/>
+      <c r="N19" s="94"/>
+      <c r="O19" s="95"/>
+      <c r="P19" s="23"/>
+      <c r="Q19" s="26"/>
       <c r="U19" s="9" t="str">
         <f>DEC2HEX(HEX2DEC(U17)+X17*1024 - 1)</f>
         <v>31FFF</v>
       </c>
-      <c r="V19" s="104"/>
-      <c r="W19" s="105"/>
-      <c r="X19" s="64"/>
+      <c r="V19" s="19"/>
+      <c r="W19" s="20"/>
+      <c r="X19" s="38"/>
     </row>
     <row r="20" spans="1:24" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A20" s="8" t="e">
         <f t="shared" ref="A20" si="24">DEC2HEX(HEX2DEC(A19)+1)</f>
         <v>#REF!</v>
       </c>
-      <c r="B20" s="55" t="s">
+      <c r="B20" s="84" t="s">
         <v>11</v>
       </c>
-      <c r="C20" s="34" t="s">
+      <c r="C20" s="106" t="s">
         <v>7</v>
       </c>
-      <c r="D20" s="31">
-        <v>4</v>
-      </c>
-      <c r="E20" s="15"/>
+      <c r="D20" s="21">
+        <v>4</v>
+      </c>
+      <c r="E20" s="66"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="8" t="str">
         <f t="shared" ref="H20" si="25">DEC2HEX(HEX2DEC(H19)+1)</f>
         <v>2F000</v>
       </c>
-      <c r="I20" s="157" t="s">
+      <c r="I20" s="124" t="s">
         <v>42</v>
       </c>
-      <c r="J20" s="158"/>
-      <c r="K20" s="63">
+      <c r="J20" s="125"/>
+      <c r="K20" s="37">
         <v>4</v>
       </c>
       <c r="M20" s="8" t="str">
         <f t="shared" si="16"/>
         <v>25000</v>
       </c>
-      <c r="N20" s="110" t="s">
-        <v>69</v>
-      </c>
-      <c r="O20" s="111"/>
-      <c r="P20" s="31">
-        <v>4</v>
-      </c>
-      <c r="Q20" s="46" t="s">
-        <v>71</v>
+      <c r="N20" s="90" t="s">
+        <v>68</v>
+      </c>
+      <c r="O20" s="91"/>
+      <c r="P20" s="21">
+        <v>4</v>
+      </c>
+      <c r="Q20" s="32" t="s">
+        <v>70</v>
       </c>
       <c r="U20" s="8" t="str">
         <f t="shared" ref="U20" si="26">DEC2HEX(HEX2DEC(U19)+1)</f>
         <v>32000</v>
       </c>
-      <c r="V20" s="114" t="s">
+      <c r="V20" s="112" t="s">
         <v>60</v>
       </c>
-      <c r="W20" s="115"/>
-      <c r="X20" s="63">
+      <c r="W20" s="113"/>
+      <c r="X20" s="37">
         <v>8</v>
       </c>
     </row>
@@ -2399,235 +2395,235 @@
       <c r="A21" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B21" s="56"/>
-      <c r="C21" s="58"/>
-      <c r="D21" s="32"/>
-      <c r="E21" s="16"/>
+      <c r="B21" s="85"/>
+      <c r="C21" s="123"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="67"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
       <c r="H21" s="9" t="str">
         <f>DEC2HEX(HEX2DEC(H20)+K20*1024 - 1)</f>
         <v>2FFFF</v>
       </c>
-      <c r="I21" s="159"/>
-      <c r="J21" s="160"/>
-      <c r="K21" s="64"/>
+      <c r="I21" s="126"/>
+      <c r="J21" s="127"/>
+      <c r="K21" s="38"/>
       <c r="M21" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="N21" s="120"/>
-      <c r="O21" s="121"/>
-      <c r="P21" s="32"/>
-      <c r="Q21" s="47"/>
+      <c r="N21" s="92"/>
+      <c r="O21" s="93"/>
+      <c r="P21" s="22"/>
+      <c r="Q21" s="25"/>
       <c r="U21" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="V21" s="118"/>
-      <c r="W21" s="119"/>
-      <c r="X21" s="69"/>
+        <v>61</v>
+      </c>
+      <c r="V21" s="114"/>
+      <c r="W21" s="115"/>
+      <c r="X21" s="118"/>
     </row>
     <row r="22" spans="1:24" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A22" s="9" t="e">
         <f t="shared" ref="A22" si="27">DEC2HEX(HEX2DEC(A20)+D20*1024 - 1)</f>
         <v>#REF!</v>
       </c>
-      <c r="B22" s="57"/>
-      <c r="C22" s="35"/>
-      <c r="D22" s="33"/>
-      <c r="E22" s="17"/>
+      <c r="B22" s="86"/>
+      <c r="C22" s="107"/>
+      <c r="D22" s="23"/>
+      <c r="E22" s="68"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
       <c r="H22" s="8" t="str">
         <f t="shared" ref="H22" si="28">DEC2HEX(HEX2DEC(H21)+1)</f>
         <v>30000</v>
       </c>
-      <c r="I22" s="153" t="s">
+      <c r="I22" s="119" t="s">
         <v>43</v>
       </c>
-      <c r="J22" s="154"/>
-      <c r="K22" s="63">
+      <c r="J22" s="120"/>
+      <c r="K22" s="37">
         <v>4</v>
       </c>
       <c r="M22" s="9" t="str">
         <f t="shared" si="19"/>
         <v>25FFF</v>
       </c>
-      <c r="N22" s="112"/>
-      <c r="O22" s="113"/>
-      <c r="P22" s="33"/>
-      <c r="Q22" s="48"/>
+      <c r="N22" s="94"/>
+      <c r="O22" s="95"/>
+      <c r="P22" s="23"/>
+      <c r="Q22" s="26"/>
       <c r="U22" s="9" t="str">
         <f>DEC2HEX(HEX2DEC(U20)+X20*1024-1)</f>
         <v>33FFF</v>
       </c>
       <c r="V22" s="116"/>
       <c r="W22" s="117"/>
-      <c r="X22" s="64"/>
+      <c r="X22" s="38"/>
     </row>
     <row r="23" spans="1:24" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A23" s="8" t="e">
         <f>DEC2HEX(HEX2DEC(A22)+1)</f>
         <v>#REF!</v>
       </c>
-      <c r="B23" s="20" t="s">
+      <c r="B23" s="75" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="21" t="s">
+      <c r="C23" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="D23" s="22">
+      <c r="D23" s="29">
         <v>8</v>
       </c>
-      <c r="E23" s="18"/>
+      <c r="E23" s="55"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
       <c r="H23" s="9" t="str">
         <f>DEC2HEX(HEX2DEC(H22)+K22*1024 - 1)</f>
         <v>30FFF</v>
       </c>
-      <c r="I23" s="155"/>
-      <c r="J23" s="156"/>
-      <c r="K23" s="64"/>
+      <c r="I23" s="121"/>
+      <c r="J23" s="122"/>
+      <c r="K23" s="38"/>
       <c r="M23" s="8" t="str">
         <f t="shared" si="16"/>
         <v>26000</v>
       </c>
-      <c r="N23" s="20" t="s">
+      <c r="N23" s="75" t="s">
+        <v>71</v>
+      </c>
+      <c r="O23" s="101" t="s">
         <v>72</v>
       </c>
-      <c r="O23" s="36" t="s">
-        <v>73</v>
-      </c>
-      <c r="P23" s="22">
+      <c r="P23" s="29">
         <v>88</v>
       </c>
-      <c r="Q23" s="44" t="s">
-        <v>64</v>
+      <c r="Q23" s="31" t="s">
+        <v>63</v>
       </c>
       <c r="U23" s="8" t="str">
         <f>DEC2HEX(HEX2DEC(U22)+1)</f>
         <v>34000</v>
       </c>
-      <c r="V23" s="110" t="s">
-        <v>61</v>
-      </c>
-      <c r="W23" s="111"/>
-      <c r="X23" s="63">
-        <v>8</v>
+      <c r="V23" s="90" t="s">
+        <v>82</v>
+      </c>
+      <c r="W23" s="91"/>
+      <c r="X23" s="37">
+        <v>32</v>
       </c>
     </row>
     <row r="24" spans="1:24" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B24" s="20"/>
-      <c r="C24" s="21"/>
-      <c r="D24" s="22"/>
-      <c r="E24" s="18"/>
+      <c r="B24" s="75"/>
+      <c r="C24" s="30"/>
+      <c r="D24" s="29"/>
+      <c r="E24" s="55"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
       <c r="H24" s="8" t="str">
         <f t="shared" ref="H24" si="29">DEC2HEX(HEX2DEC(H23)+1)</f>
         <v>31000</v>
       </c>
-      <c r="I24" s="59" t="s">
+      <c r="I24" s="128" t="s">
         <v>44</v>
       </c>
-      <c r="J24" s="60"/>
-      <c r="K24" s="63">
+      <c r="J24" s="129"/>
+      <c r="K24" s="37">
         <v>4</v>
       </c>
       <c r="M24" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="N24" s="20"/>
-      <c r="O24" s="21"/>
-      <c r="P24" s="22"/>
-      <c r="Q24" s="44"/>
+      <c r="N24" s="75"/>
+      <c r="O24" s="30"/>
+      <c r="P24" s="29"/>
+      <c r="Q24" s="31"/>
       <c r="U24" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="V24" s="120"/>
-      <c r="W24" s="121"/>
-      <c r="X24" s="69"/>
+        <v>61</v>
+      </c>
+      <c r="V24" s="92"/>
+      <c r="W24" s="93"/>
+      <c r="X24" s="118"/>
     </row>
     <row r="25" spans="1:24" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A25" s="9" t="e">
         <f t="shared" ref="A25" si="30">DEC2HEX(HEX2DEC(A23)+D23*1024 - 1)</f>
         <v>#REF!</v>
       </c>
-      <c r="B25" s="20"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="22"/>
-      <c r="E25" s="18"/>
+      <c r="B25" s="75"/>
+      <c r="C25" s="30"/>
+      <c r="D25" s="29"/>
+      <c r="E25" s="55"/>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
       <c r="H25" s="9" t="str">
         <f>DEC2HEX(HEX2DEC(H24)+K24*1024 - 1)</f>
         <v>31FFF</v>
       </c>
-      <c r="I25" s="61"/>
-      <c r="J25" s="62"/>
-      <c r="K25" s="64"/>
+      <c r="I25" s="130"/>
+      <c r="J25" s="131"/>
+      <c r="K25" s="38"/>
       <c r="M25" s="9" t="str">
         <f t="shared" si="19"/>
         <v>3BFFF</v>
       </c>
-      <c r="N25" s="20"/>
-      <c r="O25" s="21"/>
-      <c r="P25" s="22"/>
-      <c r="Q25" s="44"/>
+      <c r="N25" s="75"/>
+      <c r="O25" s="30"/>
+      <c r="P25" s="29"/>
+      <c r="Q25" s="31"/>
       <c r="U25" s="9" t="str">
         <f>DEC2HEX(HEX2DEC(U23)+X23*1024 - 1)</f>
-        <v>35FFF</v>
-      </c>
-      <c r="V25" s="112"/>
-      <c r="W25" s="113"/>
-      <c r="X25" s="64"/>
+        <v>3BFFF</v>
+      </c>
+      <c r="V25" s="94"/>
+      <c r="W25" s="95"/>
+      <c r="X25" s="38"/>
     </row>
     <row r="26" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="8" t="e">
         <f t="shared" ref="A26" si="31">DEC2HEX(HEX2DEC(A25)+1)</f>
         <v>#REF!</v>
       </c>
-      <c r="B26" s="20" t="s">
+      <c r="B26" s="75" t="s">
         <v>11</v>
       </c>
-      <c r="C26" s="36" t="s">
+      <c r="C26" s="101" t="s">
         <v>12</v>
       </c>
-      <c r="D26" s="22">
+      <c r="D26" s="29">
         <v>8</v>
       </c>
-      <c r="E26" s="18"/>
+      <c r="E26" s="55"/>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
       <c r="H26" s="8" t="str">
         <f t="shared" ref="H26" si="32">DEC2HEX(HEX2DEC(H25)+1)</f>
         <v>32000</v>
       </c>
-      <c r="I26" s="149" t="s">
+      <c r="I26" s="102" t="s">
         <v>45</v>
       </c>
-      <c r="J26" s="150"/>
-      <c r="K26" s="63">
+      <c r="J26" s="103"/>
+      <c r="K26" s="37">
         <v>4</v>
       </c>
       <c r="M26" s="8" t="str">
         <f t="shared" si="16"/>
         <v>3C000</v>
       </c>
-      <c r="N26" s="55" t="s">
+      <c r="N26" s="84" t="s">
         <v>24</v>
       </c>
-      <c r="O26" s="142" t="s">
+      <c r="O26" s="87" t="s">
         <v>28</v>
       </c>
-      <c r="P26" s="31">
+      <c r="P26" s="21">
         <v>8</v>
       </c>
-      <c r="Q26" s="46" t="s">
-        <v>65</v>
+      <c r="Q26" s="32" t="s">
+        <v>64</v>
       </c>
       <c r="U26"/>
     </row>
@@ -2635,26 +2631,26 @@
       <c r="A27" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="20"/>
-      <c r="C27" s="21"/>
-      <c r="D27" s="22"/>
-      <c r="E27" s="18"/>
+      <c r="B27" s="75"/>
+      <c r="C27" s="30"/>
+      <c r="D27" s="29"/>
+      <c r="E27" s="55"/>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
       <c r="H27" s="9" t="str">
         <f>DEC2HEX(HEX2DEC(H26)+K26*1024 - 1)</f>
         <v>32FFF</v>
       </c>
-      <c r="I27" s="151"/>
-      <c r="J27" s="152"/>
-      <c r="K27" s="64"/>
+      <c r="I27" s="104"/>
+      <c r="J27" s="105"/>
+      <c r="K27" s="38"/>
       <c r="M27" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="N27" s="56"/>
-      <c r="O27" s="143"/>
-      <c r="P27" s="32"/>
-      <c r="Q27" s="47"/>
+      <c r="N27" s="85"/>
+      <c r="O27" s="88"/>
+      <c r="P27" s="22"/>
+      <c r="Q27" s="25"/>
       <c r="U27"/>
     </row>
     <row r="28" spans="1:24" ht="15.75" x14ac:dyDescent="0.2">
@@ -2662,31 +2658,31 @@
         <f t="shared" ref="A28" si="33">DEC2HEX(HEX2DEC(A26)+D26*1024 - 1)</f>
         <v>#REF!</v>
       </c>
-      <c r="B28" s="20"/>
-      <c r="C28" s="21"/>
-      <c r="D28" s="22"/>
-      <c r="E28" s="18"/>
+      <c r="B28" s="75"/>
+      <c r="C28" s="30"/>
+      <c r="D28" s="29"/>
+      <c r="E28" s="55"/>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
       <c r="H28" s="8" t="str">
         <f t="shared" ref="H28:H42" si="34">DEC2HEX(HEX2DEC(H27)+1)</f>
         <v>33000</v>
       </c>
-      <c r="I28" s="145" t="s">
+      <c r="I28" s="96" t="s">
         <v>46</v>
       </c>
-      <c r="J28" s="146"/>
-      <c r="K28" s="63">
+      <c r="J28" s="97"/>
+      <c r="K28" s="37">
         <v>4</v>
       </c>
       <c r="M28" s="9" t="str">
         <f t="shared" si="19"/>
         <v>3DFFF</v>
       </c>
-      <c r="N28" s="57"/>
-      <c r="O28" s="144"/>
-      <c r="P28" s="33"/>
-      <c r="Q28" s="48"/>
+      <c r="N28" s="86"/>
+      <c r="O28" s="89"/>
+      <c r="P28" s="23"/>
+      <c r="Q28" s="26"/>
       <c r="U28"/>
     </row>
     <row r="29" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2694,15 +2690,15 @@
         <f t="shared" ref="A29" si="35">DEC2HEX(HEX2DEC(A28)+1)</f>
         <v>#REF!</v>
       </c>
-      <c r="B29" s="19" t="e">
+      <c r="B29" s="100" t="e">
         <f>CONCATENATE("CFG_TELINK_SDK_TYPE: ",A29)</f>
         <v>#REF!</v>
       </c>
-      <c r="C29" s="19"/>
-      <c r="D29" s="22">
-        <v>4</v>
-      </c>
-      <c r="E29" s="18" t="s">
+      <c r="C29" s="100"/>
+      <c r="D29" s="29">
+        <v>4</v>
+      </c>
+      <c r="E29" s="55" t="s">
         <v>18</v>
       </c>
       <c r="F29" s="1"/>
@@ -2711,24 +2707,24 @@
         <f>DEC2HEX(HEX2DEC(H28)+K28*1024 - 1)</f>
         <v>33FFF</v>
       </c>
-      <c r="I29" s="147"/>
-      <c r="J29" s="148"/>
-      <c r="K29" s="64"/>
+      <c r="I29" s="98"/>
+      <c r="J29" s="99"/>
+      <c r="K29" s="38"/>
       <c r="M29" s="8" t="str">
         <f t="shared" si="16"/>
         <v>3E000</v>
       </c>
-      <c r="N29" s="170" t="s">
+      <c r="N29" s="69" t="s">
         <v>24</v>
       </c>
-      <c r="O29" s="173" t="s">
+      <c r="O29" s="72" t="s">
         <v>28</v>
       </c>
-      <c r="P29" s="31">
+      <c r="P29" s="21">
         <v>8</v>
       </c>
-      <c r="Q29" s="46" t="s">
-        <v>66</v>
+      <c r="Q29" s="32" t="s">
+        <v>65</v>
       </c>
       <c r="U29"/>
     </row>
@@ -2737,31 +2733,31 @@
         <v>0</v>
       </c>
       <c r="B30" s="3"/>
-      <c r="C30" s="34" t="s">
+      <c r="C30" s="106" t="s">
         <v>22</v>
       </c>
-      <c r="D30" s="22"/>
-      <c r="E30" s="18"/>
+      <c r="D30" s="29"/>
+      <c r="E30" s="55"/>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
       <c r="H30" s="8" t="str">
         <f t="shared" si="34"/>
         <v>34000</v>
       </c>
-      <c r="I30" s="138" t="s">
+      <c r="I30" s="108" t="s">
         <v>47</v>
       </c>
-      <c r="J30" s="139"/>
-      <c r="K30" s="63">
+      <c r="J30" s="109"/>
+      <c r="K30" s="37">
         <v>4</v>
       </c>
       <c r="M30" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="N30" s="171"/>
-      <c r="O30" s="174"/>
-      <c r="P30" s="32"/>
-      <c r="Q30" s="47"/>
+      <c r="N30" s="70"/>
+      <c r="O30" s="73"/>
+      <c r="P30" s="22"/>
+      <c r="Q30" s="25"/>
       <c r="U30"/>
     </row>
     <row r="31" spans="1:24" ht="15.75" x14ac:dyDescent="0.2">
@@ -2770,26 +2766,26 @@
         <v>#REF!</v>
       </c>
       <c r="B31" s="4"/>
-      <c r="C31" s="35"/>
-      <c r="D31" s="22"/>
-      <c r="E31" s="18"/>
+      <c r="C31" s="107"/>
+      <c r="D31" s="29"/>
+      <c r="E31" s="55"/>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
       <c r="H31" s="9" t="str">
         <f t="shared" ref="H31" si="37">DEC2HEX(HEX2DEC(H30)+K30*1024 - 1)</f>
         <v>34FFF</v>
       </c>
-      <c r="I31" s="140"/>
-      <c r="J31" s="141"/>
-      <c r="K31" s="64"/>
+      <c r="I31" s="110"/>
+      <c r="J31" s="111"/>
+      <c r="K31" s="38"/>
       <c r="M31" s="9" t="str">
         <f t="shared" si="19"/>
         <v>3FFFF</v>
       </c>
-      <c r="N31" s="172"/>
-      <c r="O31" s="175"/>
-      <c r="P31" s="33"/>
-      <c r="Q31" s="48"/>
+      <c r="N31" s="71"/>
+      <c r="O31" s="74"/>
+      <c r="P31" s="23"/>
+      <c r="Q31" s="26"/>
       <c r="U31"/>
     </row>
     <row r="32" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2797,16 +2793,16 @@
         <f t="shared" ref="A32" si="38">DEC2HEX(HEX2DEC(A31)+1)</f>
         <v>#REF!</v>
       </c>
-      <c r="B32" s="20" t="s">
+      <c r="B32" s="75" t="s">
         <v>20</v>
       </c>
-      <c r="C32" s="21" t="s">
+      <c r="C32" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="D32" s="22">
-        <v>4</v>
-      </c>
-      <c r="E32" s="18" t="s">
+      <c r="D32" s="29">
+        <v>4</v>
+      </c>
+      <c r="E32" s="55" t="s">
         <v>21</v>
       </c>
       <c r="F32" s="1"/>
@@ -2815,25 +2811,25 @@
         <f t="shared" si="34"/>
         <v>35000</v>
       </c>
-      <c r="I32" s="161" t="s">
+      <c r="I32" s="76" t="s">
         <v>48</v>
       </c>
-      <c r="J32" s="162"/>
-      <c r="K32" s="63">
+      <c r="J32" s="77"/>
+      <c r="K32" s="37">
         <v>4</v>
       </c>
       <c r="M32" s="8" t="str">
         <f t="shared" si="16"/>
         <v>40000</v>
       </c>
-      <c r="N32" s="25" t="s">
+      <c r="N32" s="60" t="s">
         <v>29</v>
       </c>
-      <c r="O32" s="26"/>
-      <c r="P32" s="31">
+      <c r="O32" s="61"/>
+      <c r="P32" s="21">
         <v>256</v>
       </c>
-      <c r="Q32" s="46" t="s">
+      <c r="Q32" s="32" t="s">
         <v>29</v>
       </c>
       <c r="U32"/>
@@ -2842,26 +2838,26 @@
       <c r="A33" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B33" s="20"/>
-      <c r="C33" s="21"/>
-      <c r="D33" s="22"/>
-      <c r="E33" s="18"/>
+      <c r="B33" s="75"/>
+      <c r="C33" s="30"/>
+      <c r="D33" s="29"/>
+      <c r="E33" s="55"/>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
       <c r="H33" s="9" t="str">
         <f t="shared" ref="H33" si="39">DEC2HEX(HEX2DEC(H32)+K32*1024 - 1)</f>
         <v>35FFF</v>
       </c>
-      <c r="I33" s="163"/>
-      <c r="J33" s="164"/>
-      <c r="K33" s="64"/>
+      <c r="I33" s="78"/>
+      <c r="J33" s="79"/>
+      <c r="K33" s="38"/>
       <c r="M33" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="N33" s="27"/>
-      <c r="O33" s="28"/>
-      <c r="P33" s="32"/>
-      <c r="Q33" s="47"/>
+      <c r="N33" s="62"/>
+      <c r="O33" s="63"/>
+      <c r="P33" s="22"/>
+      <c r="Q33" s="25"/>
       <c r="U33"/>
     </row>
     <row r="34" spans="1:21" ht="15.75" x14ac:dyDescent="0.2">
@@ -2869,31 +2865,31 @@
         <f t="shared" ref="A34" si="40">DEC2HEX(HEX2DEC(A32)+D32*1024 - 1)</f>
         <v>#REF!</v>
       </c>
-      <c r="B34" s="20"/>
-      <c r="C34" s="21"/>
-      <c r="D34" s="22"/>
-      <c r="E34" s="18"/>
+      <c r="B34" s="75"/>
+      <c r="C34" s="30"/>
+      <c r="D34" s="29"/>
+      <c r="E34" s="55"/>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
       <c r="H34" s="8" t="str">
         <f t="shared" si="34"/>
         <v>36000</v>
       </c>
-      <c r="I34" s="65" t="s">
+      <c r="I34" s="49" t="s">
         <v>49</v>
       </c>
-      <c r="J34" s="66"/>
-      <c r="K34" s="63">
+      <c r="J34" s="50"/>
+      <c r="K34" s="37">
         <v>4</v>
       </c>
       <c r="M34" s="9" t="str">
         <f t="shared" si="19"/>
         <v>7FFFF</v>
       </c>
-      <c r="N34" s="29"/>
-      <c r="O34" s="30"/>
-      <c r="P34" s="33"/>
-      <c r="Q34" s="48"/>
+      <c r="N34" s="64"/>
+      <c r="O34" s="65"/>
+      <c r="P34" s="23"/>
+      <c r="Q34" s="26"/>
       <c r="U34"/>
     </row>
     <row r="35" spans="1:21" ht="15.75" x14ac:dyDescent="0.2">
@@ -2901,33 +2897,33 @@
         <f t="shared" ref="A35" si="41">DEC2HEX(HEX2DEC(A34)+1)</f>
         <v>#REF!</v>
       </c>
-      <c r="B35" s="25" t="s">
+      <c r="B35" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="C35" s="26"/>
-      <c r="D35" s="31">
-        <v>4</v>
-      </c>
-      <c r="E35" s="15"/>
+      <c r="C35" s="61"/>
+      <c r="D35" s="21">
+        <v>4</v>
+      </c>
+      <c r="E35" s="66"/>
       <c r="H35" s="9" t="str">
         <f t="shared" ref="H35" si="42">DEC2HEX(HEX2DEC(H34)+K34*1024 - 1)</f>
         <v>36FFF</v>
       </c>
-      <c r="I35" s="67"/>
-      <c r="J35" s="68"/>
-      <c r="K35" s="64"/>
+      <c r="I35" s="51"/>
+      <c r="J35" s="52"/>
+      <c r="K35" s="38"/>
       <c r="M35" s="8" t="str">
         <f t="shared" si="16"/>
         <v>80000</v>
       </c>
-      <c r="N35" s="49" t="s">
+      <c r="N35" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="O35" s="50"/>
-      <c r="P35" s="22">
+      <c r="O35" s="40"/>
+      <c r="P35" s="29">
         <v>256</v>
       </c>
-      <c r="Q35" s="44" t="s">
+      <c r="Q35" s="31" t="s">
         <v>32</v>
       </c>
       <c r="U35"/>
@@ -2936,28 +2932,28 @@
       <c r="A36" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B36" s="27"/>
-      <c r="C36" s="28"/>
-      <c r="D36" s="32"/>
-      <c r="E36" s="16"/>
+      <c r="B36" s="62"/>
+      <c r="C36" s="63"/>
+      <c r="D36" s="22"/>
+      <c r="E36" s="67"/>
       <c r="H36" s="8" t="str">
         <f t="shared" si="34"/>
         <v>37000</v>
       </c>
-      <c r="I36" s="130" t="s">
+      <c r="I36" s="80" t="s">
         <v>50</v>
       </c>
-      <c r="J36" s="131"/>
-      <c r="K36" s="63">
+      <c r="J36" s="81"/>
+      <c r="K36" s="37">
         <v>4</v>
       </c>
       <c r="M36" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="N36" s="51"/>
-      <c r="O36" s="52"/>
-      <c r="P36" s="22"/>
-      <c r="Q36" s="44"/>
+      <c r="N36" s="41"/>
+      <c r="O36" s="42"/>
+      <c r="P36" s="29"/>
+      <c r="Q36" s="31"/>
       <c r="U36"/>
     </row>
     <row r="37" spans="1:21" ht="15.75" x14ac:dyDescent="0.2">
@@ -2965,25 +2961,25 @@
         <f t="shared" ref="A37" si="43">DEC2HEX(HEX2DEC(A35)+D35*1024 - 1)</f>
         <v>#REF!</v>
       </c>
-      <c r="B37" s="29"/>
-      <c r="C37" s="30"/>
-      <c r="D37" s="33"/>
-      <c r="E37" s="17"/>
+      <c r="B37" s="64"/>
+      <c r="C37" s="65"/>
+      <c r="D37" s="23"/>
+      <c r="E37" s="68"/>
       <c r="H37" s="9" t="str">
         <f t="shared" ref="H37" si="44">DEC2HEX(HEX2DEC(H36)+K36*1024 - 1)</f>
         <v>37FFF</v>
       </c>
-      <c r="I37" s="132"/>
-      <c r="J37" s="133"/>
-      <c r="K37" s="64"/>
+      <c r="I37" s="82"/>
+      <c r="J37" s="83"/>
+      <c r="K37" s="38"/>
       <c r="M37" s="9" t="str">
         <f t="shared" si="19"/>
         <v>BFFFF</v>
       </c>
-      <c r="N37" s="53"/>
-      <c r="O37" s="54"/>
-      <c r="P37" s="22"/>
-      <c r="Q37" s="44"/>
+      <c r="N37" s="43"/>
+      <c r="O37" s="44"/>
+      <c r="P37" s="29"/>
+      <c r="Q37" s="31"/>
       <c r="U37"/>
     </row>
     <row r="38" spans="1:21" ht="15.75" x14ac:dyDescent="0.2">
@@ -2991,37 +2987,37 @@
         <f t="shared" ref="A38" si="45">DEC2HEX(HEX2DEC(A37)+1)</f>
         <v>#REF!</v>
       </c>
-      <c r="B38" s="23" t="s">
+      <c r="B38" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="C38" s="24"/>
-      <c r="D38" s="22">
-        <v>4</v>
-      </c>
-      <c r="E38" s="18"/>
+      <c r="C38" s="54"/>
+      <c r="D38" s="29">
+        <v>4</v>
+      </c>
+      <c r="E38" s="55"/>
       <c r="H38" s="8" t="str">
         <f t="shared" si="34"/>
         <v>38000</v>
       </c>
-      <c r="I38" s="134" t="s">
+      <c r="I38" s="56" t="s">
         <v>51</v>
       </c>
-      <c r="J38" s="135"/>
-      <c r="K38" s="63">
+      <c r="J38" s="57"/>
+      <c r="K38" s="37">
         <v>4</v>
       </c>
       <c r="M38" s="8" t="str">
         <f t="shared" si="16"/>
         <v>C0000</v>
       </c>
-      <c r="N38" s="21" t="s">
+      <c r="N38" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="O38" s="21"/>
-      <c r="P38" s="22">
+      <c r="O38" s="30"/>
+      <c r="P38" s="29">
         <v>248</v>
       </c>
-      <c r="Q38" s="44" t="s">
+      <c r="Q38" s="31" t="s">
         <v>32</v>
       </c>
       <c r="U38"/>
@@ -3030,24 +3026,24 @@
       <c r="A39" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B39" s="24"/>
-      <c r="C39" s="24"/>
-      <c r="D39" s="22"/>
-      <c r="E39" s="18"/>
+      <c r="B39" s="54"/>
+      <c r="C39" s="54"/>
+      <c r="D39" s="29"/>
+      <c r="E39" s="55"/>
       <c r="H39" s="9" t="str">
         <f t="shared" ref="H39" si="46">DEC2HEX(HEX2DEC(H38)+K38*1024 - 1)</f>
         <v>38FFF</v>
       </c>
-      <c r="I39" s="136"/>
-      <c r="J39" s="137"/>
-      <c r="K39" s="64"/>
+      <c r="I39" s="58"/>
+      <c r="J39" s="59"/>
+      <c r="K39" s="38"/>
       <c r="M39" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="N39" s="21"/>
-      <c r="O39" s="21"/>
-      <c r="P39" s="22"/>
-      <c r="Q39" s="44"/>
+      <c r="N39" s="30"/>
+      <c r="O39" s="30"/>
+      <c r="P39" s="29"/>
+      <c r="Q39" s="31"/>
       <c r="U39"/>
     </row>
     <row r="40" spans="1:21" ht="15.75" x14ac:dyDescent="0.2">
@@ -3055,29 +3051,29 @@
         <f t="shared" ref="A40" si="47">DEC2HEX(HEX2DEC(A38)+D38*1024 - 1)</f>
         <v>#REF!</v>
       </c>
-      <c r="B40" s="24"/>
-      <c r="C40" s="24"/>
-      <c r="D40" s="22"/>
-      <c r="E40" s="18"/>
+      <c r="B40" s="54"/>
+      <c r="C40" s="54"/>
+      <c r="D40" s="29"/>
+      <c r="E40" s="55"/>
       <c r="H40" s="8" t="str">
         <f t="shared" si="34"/>
         <v>39000</v>
       </c>
-      <c r="I40" s="122" t="s">
+      <c r="I40" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="J40" s="123"/>
-      <c r="K40" s="63">
+      <c r="J40" s="34"/>
+      <c r="K40" s="37">
         <v>4</v>
       </c>
       <c r="M40" s="9" t="str">
         <f t="shared" si="19"/>
         <v>FDFFF</v>
       </c>
-      <c r="N40" s="21"/>
-      <c r="O40" s="21"/>
-      <c r="P40" s="22"/>
-      <c r="Q40" s="44"/>
+      <c r="N40" s="30"/>
+      <c r="O40" s="30"/>
+      <c r="P40" s="29"/>
+      <c r="Q40" s="31"/>
       <c r="U40"/>
     </row>
     <row r="41" spans="1:21" ht="15.75" x14ac:dyDescent="0.2">
@@ -3085,22 +3081,22 @@
         <f t="shared" ref="H41" si="48">DEC2HEX(HEX2DEC(H40)+K40*1024 - 1)</f>
         <v>39FFF</v>
       </c>
-      <c r="I41" s="124"/>
-      <c r="J41" s="125"/>
-      <c r="K41" s="64"/>
+      <c r="I41" s="35"/>
+      <c r="J41" s="36"/>
+      <c r="K41" s="38"/>
       <c r="M41" s="8" t="str">
         <f t="shared" si="16"/>
         <v>FE000</v>
       </c>
-      <c r="N41" s="168" t="s">
-        <v>74</v>
-      </c>
-      <c r="O41" s="101"/>
-      <c r="P41" s="31">
-        <v>4</v>
-      </c>
-      <c r="Q41" s="169" t="s">
-        <v>76</v>
+      <c r="N41" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="O41" s="16"/>
+      <c r="P41" s="21">
+        <v>4</v>
+      </c>
+      <c r="Q41" s="24" t="s">
+        <v>75</v>
       </c>
       <c r="U41"/>
     </row>
@@ -3109,20 +3105,20 @@
         <f t="shared" si="34"/>
         <v>3A000</v>
       </c>
-      <c r="I42" s="126" t="s">
+      <c r="I42" s="45" t="s">
         <v>53</v>
       </c>
-      <c r="J42" s="127"/>
-      <c r="K42" s="63">
+      <c r="J42" s="46"/>
+      <c r="K42" s="37">
         <v>4</v>
       </c>
       <c r="M42" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="N42" s="102"/>
-      <c r="O42" s="103"/>
-      <c r="P42" s="32"/>
-      <c r="Q42" s="47"/>
+      <c r="N42" s="17"/>
+      <c r="O42" s="18"/>
+      <c r="P42" s="22"/>
+      <c r="Q42" s="25"/>
       <c r="U42"/>
     </row>
     <row r="43" spans="1:21" ht="15.75" x14ac:dyDescent="0.2">
@@ -3130,17 +3126,17 @@
         <f t="shared" ref="H43" si="49">DEC2HEX(HEX2DEC(H42)+K42*1024 - 1)</f>
         <v>3AFFF</v>
       </c>
-      <c r="I43" s="128"/>
-      <c r="J43" s="129"/>
-      <c r="K43" s="64"/>
+      <c r="I43" s="47"/>
+      <c r="J43" s="48"/>
+      <c r="K43" s="38"/>
       <c r="M43" s="9" t="str">
         <f t="shared" si="19"/>
         <v>FEFFF</v>
       </c>
-      <c r="N43" s="104"/>
-      <c r="O43" s="105"/>
-      <c r="P43" s="33"/>
-      <c r="Q43" s="48"/>
+      <c r="N43" s="19"/>
+      <c r="O43" s="20"/>
+      <c r="P43" s="23"/>
+      <c r="Q43" s="26"/>
       <c r="U43"/>
     </row>
     <row r="44" spans="1:21" ht="15.75" x14ac:dyDescent="0.2">
@@ -3149,15 +3145,15 @@
         <f t="shared" si="16"/>
         <v>FF000</v>
       </c>
-      <c r="N44" s="165" t="s">
-        <v>75</v>
-      </c>
-      <c r="O44" s="166"/>
-      <c r="P44" s="22">
-        <v>4</v>
-      </c>
-      <c r="Q44" s="169" t="s">
-        <v>82</v>
+      <c r="N44" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="O44" s="28"/>
+      <c r="P44" s="29">
+        <v>4</v>
+      </c>
+      <c r="Q44" s="24" t="s">
+        <v>81</v>
       </c>
       <c r="U44"/>
     </row>
@@ -3166,10 +3162,10 @@
       <c r="M45" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="N45" s="166"/>
-      <c r="O45" s="166"/>
-      <c r="P45" s="22"/>
-      <c r="Q45" s="47"/>
+      <c r="N45" s="28"/>
+      <c r="O45" s="28"/>
+      <c r="P45" s="29"/>
+      <c r="Q45" s="25"/>
       <c r="U45"/>
     </row>
     <row r="46" spans="1:21" ht="15.75" x14ac:dyDescent="0.2">
@@ -3177,10 +3173,10 @@
         <f t="shared" si="19"/>
         <v>FFFFF</v>
       </c>
-      <c r="N46" s="166"/>
-      <c r="O46" s="166"/>
-      <c r="P46" s="22"/>
-      <c r="Q46" s="48"/>
+      <c r="N46" s="28"/>
+      <c r="O46" s="28"/>
+      <c r="P46" s="29"/>
+      <c r="Q46" s="26"/>
       <c r="U46"/>
     </row>
     <row r="47" spans="1:21" x14ac:dyDescent="0.2">
@@ -3218,24 +3214,121 @@
     </row>
   </sheetData>
   <mergeCells count="157">
-    <mergeCell ref="N41:O43"/>
-    <mergeCell ref="P41:P43"/>
-    <mergeCell ref="Q41:Q43"/>
-    <mergeCell ref="N44:O46"/>
-    <mergeCell ref="P44:P46"/>
-    <mergeCell ref="Q44:Q46"/>
-    <mergeCell ref="N38:O40"/>
-    <mergeCell ref="P38:P40"/>
-    <mergeCell ref="Q38:Q40"/>
-    <mergeCell ref="P32:P34"/>
-    <mergeCell ref="Q32:Q34"/>
-    <mergeCell ref="I40:J41"/>
-    <mergeCell ref="K40:K41"/>
-    <mergeCell ref="N35:O37"/>
-    <mergeCell ref="P35:P37"/>
-    <mergeCell ref="Q35:Q37"/>
-    <mergeCell ref="I42:J43"/>
-    <mergeCell ref="K42:K43"/>
+    <mergeCell ref="P2:P4"/>
+    <mergeCell ref="Q2:Q4"/>
+    <mergeCell ref="V2:W4"/>
+    <mergeCell ref="X2:X4"/>
+    <mergeCell ref="I4:J5"/>
+    <mergeCell ref="K4:K5"/>
+    <mergeCell ref="V5:W7"/>
+    <mergeCell ref="X5:X7"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="V1:W1"/>
+    <mergeCell ref="B2:C4"/>
+    <mergeCell ref="D2:D4"/>
+    <mergeCell ref="E2:E4"/>
+    <mergeCell ref="I2:J3"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="N2:O4"/>
+    <mergeCell ref="B5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="N5:O7"/>
+    <mergeCell ref="P5:P7"/>
+    <mergeCell ref="Q5:Q7"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="V8:W10"/>
+    <mergeCell ref="X8:X10"/>
+    <mergeCell ref="I10:J11"/>
+    <mergeCell ref="K10:K11"/>
+    <mergeCell ref="V11:W13"/>
+    <mergeCell ref="X11:X13"/>
+    <mergeCell ref="B8:C10"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="E8:E10"/>
+    <mergeCell ref="I8:J9"/>
+    <mergeCell ref="K8:K9"/>
+    <mergeCell ref="N8:O10"/>
+    <mergeCell ref="B11:C13"/>
+    <mergeCell ref="D11:D13"/>
+    <mergeCell ref="E11:E13"/>
+    <mergeCell ref="N11:O13"/>
+    <mergeCell ref="P11:P13"/>
+    <mergeCell ref="Q11:Q13"/>
+    <mergeCell ref="I12:J13"/>
+    <mergeCell ref="K12:K13"/>
+    <mergeCell ref="P8:P10"/>
+    <mergeCell ref="Q8:Q10"/>
+    <mergeCell ref="V14:W16"/>
+    <mergeCell ref="X14:X16"/>
+    <mergeCell ref="I16:J17"/>
+    <mergeCell ref="K16:K17"/>
+    <mergeCell ref="V17:W19"/>
+    <mergeCell ref="X17:X19"/>
+    <mergeCell ref="I6:J7"/>
+    <mergeCell ref="K6:K7"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="C14:C16"/>
+    <mergeCell ref="D14:D16"/>
+    <mergeCell ref="E14:E16"/>
+    <mergeCell ref="I14:J15"/>
+    <mergeCell ref="K14:K15"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="C17:C19"/>
+    <mergeCell ref="D17:D19"/>
+    <mergeCell ref="E17:E19"/>
+    <mergeCell ref="I18:J19"/>
+    <mergeCell ref="K18:K19"/>
+    <mergeCell ref="Q14:Q16"/>
+    <mergeCell ref="V20:W22"/>
+    <mergeCell ref="X20:X22"/>
+    <mergeCell ref="I22:J23"/>
+    <mergeCell ref="K22:K23"/>
+    <mergeCell ref="Q17:Q19"/>
+    <mergeCell ref="V23:W25"/>
+    <mergeCell ref="X23:X25"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="D20:D22"/>
+    <mergeCell ref="E20:E22"/>
+    <mergeCell ref="I20:J21"/>
+    <mergeCell ref="K20:K21"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="C23:C25"/>
+    <mergeCell ref="D23:D25"/>
+    <mergeCell ref="E23:E25"/>
+    <mergeCell ref="N17:O19"/>
+    <mergeCell ref="P17:P19"/>
+    <mergeCell ref="I24:J25"/>
+    <mergeCell ref="K24:K25"/>
+    <mergeCell ref="N14:O16"/>
+    <mergeCell ref="P14:P16"/>
+    <mergeCell ref="N26:N28"/>
+    <mergeCell ref="O26:O28"/>
+    <mergeCell ref="P26:P28"/>
+    <mergeCell ref="N20:O22"/>
+    <mergeCell ref="P20:P22"/>
+    <mergeCell ref="Q20:Q22"/>
+    <mergeCell ref="I28:J29"/>
+    <mergeCell ref="K28:K29"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="D29:D31"/>
+    <mergeCell ref="E29:E31"/>
+    <mergeCell ref="N23:N25"/>
+    <mergeCell ref="O23:O25"/>
+    <mergeCell ref="B26:B28"/>
+    <mergeCell ref="C26:C28"/>
+    <mergeCell ref="D26:D28"/>
+    <mergeCell ref="E26:E28"/>
+    <mergeCell ref="I26:J27"/>
+    <mergeCell ref="K26:K27"/>
+    <mergeCell ref="P23:P25"/>
+    <mergeCell ref="Q23:Q25"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="I30:J31"/>
+    <mergeCell ref="K30:K31"/>
     <mergeCell ref="Q26:Q28"/>
     <mergeCell ref="I34:J35"/>
     <mergeCell ref="K34:K35"/>
@@ -3260,121 +3353,24 @@
     <mergeCell ref="I36:J37"/>
     <mergeCell ref="K36:K37"/>
     <mergeCell ref="K32:K33"/>
-    <mergeCell ref="N26:N28"/>
-    <mergeCell ref="O26:O28"/>
-    <mergeCell ref="P26:P28"/>
-    <mergeCell ref="N20:O22"/>
-    <mergeCell ref="P20:P22"/>
-    <mergeCell ref="Q20:Q22"/>
-    <mergeCell ref="I28:J29"/>
-    <mergeCell ref="K28:K29"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="D29:D31"/>
-    <mergeCell ref="E29:E31"/>
-    <mergeCell ref="N23:N25"/>
-    <mergeCell ref="O23:O25"/>
-    <mergeCell ref="B26:B28"/>
-    <mergeCell ref="C26:C28"/>
-    <mergeCell ref="D26:D28"/>
-    <mergeCell ref="E26:E28"/>
-    <mergeCell ref="I26:J27"/>
-    <mergeCell ref="K26:K27"/>
-    <mergeCell ref="P23:P25"/>
-    <mergeCell ref="Q23:Q25"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="I30:J31"/>
-    <mergeCell ref="K30:K31"/>
-    <mergeCell ref="Q14:Q16"/>
-    <mergeCell ref="V20:W22"/>
-    <mergeCell ref="X20:X22"/>
-    <mergeCell ref="I22:J23"/>
-    <mergeCell ref="K22:K23"/>
-    <mergeCell ref="Q17:Q19"/>
-    <mergeCell ref="V23:W25"/>
-    <mergeCell ref="X23:X25"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="D20:D22"/>
-    <mergeCell ref="E20:E22"/>
-    <mergeCell ref="I20:J21"/>
-    <mergeCell ref="K20:K21"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="C23:C25"/>
-    <mergeCell ref="D23:D25"/>
-    <mergeCell ref="E23:E25"/>
-    <mergeCell ref="N17:O19"/>
-    <mergeCell ref="P17:P19"/>
-    <mergeCell ref="I24:J25"/>
-    <mergeCell ref="K24:K25"/>
-    <mergeCell ref="N14:O16"/>
-    <mergeCell ref="P14:P16"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="C14:C16"/>
-    <mergeCell ref="D14:D16"/>
-    <mergeCell ref="E14:E16"/>
-    <mergeCell ref="I14:J15"/>
-    <mergeCell ref="K14:K15"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="C17:C19"/>
-    <mergeCell ref="D17:D19"/>
-    <mergeCell ref="E17:E19"/>
-    <mergeCell ref="I18:J19"/>
-    <mergeCell ref="K18:K19"/>
-    <mergeCell ref="Q8:Q10"/>
-    <mergeCell ref="V14:W16"/>
-    <mergeCell ref="X14:X16"/>
-    <mergeCell ref="I16:J17"/>
-    <mergeCell ref="K16:K17"/>
-    <mergeCell ref="V17:W19"/>
-    <mergeCell ref="X17:X19"/>
-    <mergeCell ref="I6:J7"/>
-    <mergeCell ref="K6:K7"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="V8:W10"/>
-    <mergeCell ref="X8:X10"/>
-    <mergeCell ref="I10:J11"/>
-    <mergeCell ref="K10:K11"/>
-    <mergeCell ref="V11:W13"/>
-    <mergeCell ref="X11:X13"/>
-    <mergeCell ref="B8:C10"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="E8:E10"/>
-    <mergeCell ref="I8:J9"/>
-    <mergeCell ref="K8:K9"/>
-    <mergeCell ref="N8:O10"/>
-    <mergeCell ref="B11:C13"/>
-    <mergeCell ref="D11:D13"/>
-    <mergeCell ref="E11:E13"/>
-    <mergeCell ref="N11:O13"/>
-    <mergeCell ref="P11:P13"/>
-    <mergeCell ref="Q11:Q13"/>
-    <mergeCell ref="I12:J13"/>
-    <mergeCell ref="K12:K13"/>
-    <mergeCell ref="P8:P10"/>
-    <mergeCell ref="P2:P4"/>
-    <mergeCell ref="Q2:Q4"/>
-    <mergeCell ref="V2:W4"/>
-    <mergeCell ref="X2:X4"/>
-    <mergeCell ref="I4:J5"/>
-    <mergeCell ref="K4:K5"/>
-    <mergeCell ref="V5:W7"/>
-    <mergeCell ref="X5:X7"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="N1:O1"/>
-    <mergeCell ref="V1:W1"/>
-    <mergeCell ref="B2:C4"/>
-    <mergeCell ref="D2:D4"/>
-    <mergeCell ref="E2:E4"/>
-    <mergeCell ref="I2:J3"/>
-    <mergeCell ref="K2:K3"/>
-    <mergeCell ref="N2:O4"/>
-    <mergeCell ref="B5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="N5:O7"/>
-    <mergeCell ref="P5:P7"/>
-    <mergeCell ref="Q5:Q7"/>
+    <mergeCell ref="P32:P34"/>
+    <mergeCell ref="Q32:Q34"/>
+    <mergeCell ref="I40:J41"/>
+    <mergeCell ref="K40:K41"/>
+    <mergeCell ref="N35:O37"/>
+    <mergeCell ref="P35:P37"/>
+    <mergeCell ref="Q35:Q37"/>
+    <mergeCell ref="I42:J43"/>
+    <mergeCell ref="K42:K43"/>
+    <mergeCell ref="N41:O43"/>
+    <mergeCell ref="P41:P43"/>
+    <mergeCell ref="Q41:Q43"/>
+    <mergeCell ref="N44:O46"/>
+    <mergeCell ref="P44:P46"/>
+    <mergeCell ref="Q44:Q46"/>
+    <mergeCell ref="N38:O40"/>
+    <mergeCell ref="P38:P40"/>
+    <mergeCell ref="Q38:Q40"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>